<commit_message>
[이용섭] Add - [CustomerSpline/MarketLevel] 마켓 레벨에 고객 스플라인 4종 추가. Add - [GotoMarketTask/CustomerTask] 마켓 정문 앞으로 도착할 수 있는 테스트 및 기능화 작업.
</commit_message>
<xml_diff>
--- a/Content/TableData/Customer.xlsx
+++ b/Content/TableData/Customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0D4090-82FA-4CBF-9643-5441990099C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE7287-CAC0-4B71-8226-29D63F6F6897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18795" yWindow="6225" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30960" yWindow="7050" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,6 +45,9 @@
   <si>
     <t>MaxItemKind</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PathFile</t>
   </si>
 </sst>
 </file>
@@ -87,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:D12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -381,7 +387,7 @@
     <col min="3" max="4" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -394,8 +400,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -408,8 +417,11 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -422,8 +434,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -436,8 +451,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -450,8 +468,11 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -464,8 +485,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -478,8 +502,11 @@
       <c r="D7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -492,8 +519,11 @@
       <c r="D8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -506,8 +536,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -520,8 +553,11 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -534,8 +570,11 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="1">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -547,6 +586,9 @@
       </c>
       <c r="D12">
         <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>